<commit_message>
hsn sheet added in gstr1 and date format...
</commit_message>
<xml_diff>
--- a/ExcelTemplate/GSTR1_Template.xlsx
+++ b/ExcelTemplate/GSTR1_Template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="b2b" sheetId="1" r:id="rId1"/>
     <sheet name="b2cl" sheetId="2" r:id="rId2"/>
     <sheet name="b2cs" sheetId="3" r:id="rId3"/>
+    <sheet name="hsn" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Summary For B2B(4)</t>
   </si>
@@ -82,6 +83,45 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Summary For HSN(12)</t>
+  </si>
+  <si>
+    <t>No. of HSN</t>
+  </si>
+  <si>
+    <t>Total Value</t>
+  </si>
+  <si>
+    <t>Total Integrated Tax</t>
+  </si>
+  <si>
+    <t>Total Central Tax</t>
+  </si>
+  <si>
+    <t>Total State/UT Tax</t>
+  </si>
+  <si>
+    <t>HSN</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>UQC</t>
+  </si>
+  <si>
+    <t>Total Quantity</t>
+  </si>
+  <si>
+    <t>Integrated Tax Amount</t>
+  </si>
+  <si>
+    <t>Central Tax Amount</t>
+  </si>
+  <si>
+    <t>State/UT Tax Amount</t>
   </si>
 </sst>
 </file>
@@ -156,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -203,12 +243,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
@@ -331,6 +429,52 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -639,7 +783,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +1018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -949,5 +1093,138 @@
     <protectedRange sqref="B1:B3" name="Summary_1_1"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="54"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="53">
+        <f>COUNTA(A5:A1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="B3" s="43"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="53">
+        <f>SUM(E5:E1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="53">
+        <f>SUM(F5:F1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="53">
+        <f>SUM(G5:G1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="53">
+        <f>SUM(H5:H1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="53">
+        <f>SUM(I5:I1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="53">
+        <f>SUM(J5:J1048576)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>